<commit_message>
Added antennas to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elieser\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elieser\Documents\workspace\git\yard_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13455" windowHeight="7725"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="13455" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>SparkFun GPS-RTK Board - NEO-M8P-2</t>
   </si>
@@ -75,6 +75,27 @@
   </si>
   <si>
     <t>Drill mounting brackets</t>
+  </si>
+  <si>
+    <t>Interface Cable SMA to U.FL</t>
+  </si>
+  <si>
+    <t>WRL-09145</t>
+  </si>
+  <si>
+    <t>GPS/GNSS Magnetic Mount Antenna SMA - 3m</t>
+  </si>
+  <si>
+    <t>GPS-14986</t>
+  </si>
+  <si>
+    <t>GPS Antenna Ground Plate</t>
+  </si>
+  <si>
+    <t>DIY</t>
+  </si>
+  <si>
+    <t>Mast to get Base station antenna above houses</t>
   </si>
 </sst>
 </file>
@@ -82,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -125,7 +146,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,12 +431,12 @@
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -544,20 +565,48 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4.95</v>
+      </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12.95</v>
+      </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
@@ -565,6 +614,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
@@ -591,7 +643,7 @@
       </c>
       <c r="E17" s="2">
         <f>SUM(E3:E15)</f>
-        <v>916.75</v>
+        <v>952.55</v>
       </c>
     </row>
   </sheetData>
@@ -601,8 +653,11 @@
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4" display="https://www.homedepot.com/p/Ryobi-20-in-40-Volt-Brushless-Lithium-Ion-Cordless-Battery-Walk-Behind-Push-Lawn-Mower-5-0-Ah-Battery-Charger-Included-RY40180-Y/304597920"/>
     <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B12" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM to list radio prototyping needs.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="13455" windowHeight="7725"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="13455" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>SparkFun GPS-RTK Board - NEO-M8P-2</t>
-  </si>
-  <si>
-    <t>GPS-15005</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Part No.</t>
   </si>
@@ -92,10 +86,31 @@
     <t>GPS Antenna Ground Plate</t>
   </si>
   <si>
-    <t>DIY</t>
-  </si>
-  <si>
     <t>Mast to get Base station antenna above houses</t>
+  </si>
+  <si>
+    <t>First buy to test radios</t>
+  </si>
+  <si>
+    <t>GPS-15136</t>
+  </si>
+  <si>
+    <t>SparkFun GPS-RTK2 Board - ZED-F9P</t>
+  </si>
+  <si>
+    <t>GPS-15004</t>
+  </si>
+  <si>
+    <t>Pycom LoRa and Sigfox Antenna Kit - 915MHz</t>
+  </si>
+  <si>
+    <t>WRL-14676</t>
+  </si>
+  <si>
+    <t>Qwiic Cable - 100mm</t>
+  </si>
+  <si>
+    <t>PRT-14427</t>
   </si>
 </sst>
 </file>
@@ -428,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,44 +455,68 @@
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>199.95</v>
+        <v>219.95</v>
       </c>
       <c r="E3" s="2">
         <f>D3*C3</f>
-        <v>399.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>439.9</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>219.95</v>
+      </c>
+      <c r="I3" s="2">
+        <f>H3*G3</f>
+        <v>439.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -486,16 +525,26 @@
         <v>29.95</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E15" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E17" si="0">D4*C4</f>
         <v>59.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>29.95</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I17" si="1">H4*G4</f>
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -507,13 +556,20 @@
         <f t="shared" si="0"/>
         <v>39.950000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -525,13 +581,20 @@
         <f t="shared" si="0"/>
         <v>299</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <v>299</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -543,33 +606,50 @@
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>59</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -581,13 +661,23 @@
         <f t="shared" si="0"/>
         <v>9.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -599,65 +689,167 @@
         <f t="shared" si="0"/>
         <v>25.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>12.95</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.95</v>
+      </c>
       <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9.9</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>11.95</v>
+      </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
+        <v>23.9</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>11.95</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.5</v>
+      </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="2"/>
       <c r="E17" s="2">
-        <f>SUM(E3:E15)</f>
-        <v>952.55</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2">
+        <f>SUM(E3:E17)</f>
+        <v>1029.3499999999999</v>
+      </c>
+      <c r="I19" s="2">
+        <f>SUM(I3:I18)</f>
+        <v>572.39999999999986</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" display="GPS-15005"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4" display="https://www.homedepot.com/p/Ryobi-20-in-40-Volt-Brushless-Lithium-Ion-Cordless-Battery-Walk-Behind-Push-Lawn-Mower-5-0-Ah-Battery-Charger-Included-RY40180-Y/304597920"/>
     <hyperlink ref="B7" r:id="rId5"/>
     <hyperlink ref="B10" r:id="rId6"/>
     <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId8" display="DIY"/>
+    <hyperlink ref="B13" r:id="rId9"/>
+    <hyperlink ref="B14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>